<commit_message>
add colunm for colunm definition for JavaDB.
</commit_message>
<xml_diff>
--- a/src/tabledesign/INSTRUMENT.xlsx
+++ b/src/tabledesign/INSTRUMENT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>PRI</t>
   </si>
@@ -82,6 +82,13 @@
   <si>
     <t>Importing data from MassBank Record file</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>type in JavaDB</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -201,7 +208,24 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Verdana"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -359,15 +383,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル3589" displayName="テーブル3589" ref="B4:G7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B4:G7"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="name of column" dataDxfId="5"/>
-    <tableColumn id="2" name="type in mysql" dataDxfId="4"/>
-    <tableColumn id="3" name="is null?" dataDxfId="3"/>
-    <tableColumn id="4" name="is key?" dataDxfId="2"/>
-    <tableColumn id="5" name="initial value" dataDxfId="1"/>
-    <tableColumn id="6" name="description" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル3589" displayName="テーブル3589" ref="B4:H7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B4:H7"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="name of column" dataDxfId="6"/>
+    <tableColumn id="2" name="type in mysql" dataDxfId="5"/>
+    <tableColumn id="7" name="type in JavaDB" dataDxfId="0"/>
+    <tableColumn id="3" name="is null?" dataDxfId="4"/>
+    <tableColumn id="4" name="is key?" dataDxfId="3"/>
+    <tableColumn id="5" name="initial value" dataDxfId="2"/>
+    <tableColumn id="6" name="description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -671,14 +696,15 @@
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="52.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10" style="1"/>
+    <col min="4" max="4" width="19.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -686,32 +712,37 @@
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -719,17 +750,20 @@
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -737,13 +771,16 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
@@ -751,23 +788,26 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>